<commit_message>
boundary set but not ok yet
</commit_message>
<xml_diff>
--- a/backend/area_calculation_report.xlsx
+++ b/backend/area_calculation_report.xlsx
@@ -454,7 +454,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>European Measurement Code</t>
+          <t>European Union</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-12-19 12:32:05</t>
+          <t>2025-12-20 18:06:47</t>
         </is>
       </c>
     </row>

</xml_diff>